<commit_message>
added combineCharts.py and directories
</commit_message>
<xml_diff>
--- a/data/example_month_2.xlsx
+++ b/data/example_month_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerb5\vscode-projects\nfp-creighton-model-chart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6C1162-5562-4926-AC4E-77B35F872E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D79F4F-191E-4D42-A382-66E66A38C47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4515" yWindow="4125" windowWidth="21600" windowHeight="12645" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
@@ -573,7 +573,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>36892</v>
+        <v>45689</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>36893</v>
+        <v>45690</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>36894</v>
+        <v>45691</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>36895</v>
+        <v>45692</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>36896</v>
+        <v>45693</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>36897</v>
+        <v>45694</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>36898</v>
+        <v>45695</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>36899</v>
+        <v>45696</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>36900</v>
+        <v>45697</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>12</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>36901</v>
+        <v>45698</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>36902</v>
+        <v>45699</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>36903</v>
+        <v>45700</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>6</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>36904</v>
+        <v>45701</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>15</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>36905</v>
+        <v>45702</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>6</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>36906</v>
+        <v>45703</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -738,7 +738,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>36907</v>
+        <v>45704</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
@@ -749,7 +749,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>36908</v>
+        <v>45705</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>8</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>36909</v>
+        <v>45706</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>16</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2">
-        <v>36910</v>
+        <v>45707</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>13</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2">
-        <v>36911</v>
+        <v>45708</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
@@ -793,7 +793,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
-        <v>36912</v>
+        <v>45709</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>15</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2">
-        <v>36913</v>
+        <v>45710</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2">
-        <v>36914</v>
+        <v>45711</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>6</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2">
-        <v>36915</v>
+        <v>45712</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2">
-        <v>36916</v>
+        <v>45713</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>6</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2">
-        <v>36917</v>
+        <v>45714</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2">
-        <v>36918</v>
+        <v>45715</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2">
-        <v>36919</v>
+        <v>45716</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>6</v>
@@ -887,72 +887,36 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2">
-        <v>36920</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>18</v>
+        <v>45717</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2">
-        <v>36921</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>18</v>
+        <v>45718</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="2">
-        <v>36922</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="2">
-        <v>36923</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2">
-        <v>36924</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:1">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:1">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:1">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:1">
       <c r="A39" s="2"/>
     </row>
   </sheetData>

</xml_diff>